<commit_message>
Adding first and last name
</commit_message>
<xml_diff>
--- a/examples/source.xlsx
+++ b/examples/source.xlsx
@@ -12,9 +12,9 @@
     <workbookView xWindow="80" yWindow="460" windowWidth="28720" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="source.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,54 +27,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
-  <si>
-    <t>dx</t>
-  </si>
-  <si>
-    <t>user-example-com</t>
-  </si>
-  <si>
-    <t>user@example.com</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>channels</t>
+  </si>
+  <si>
+    <t>a-team</t>
+  </si>
+  <si>
+    <t>a-example-com</t>
+  </si>
+  <si>
+    <t>a@example.com</t>
+  </si>
+  <si>
+    <t>channel-a, channel-b, channel-c</t>
+  </si>
+  <si>
+    <t>b-team</t>
+  </si>
+  <si>
+    <t>b-example-com</t>
+  </si>
+  <si>
+    <t>b@example.com</t>
   </si>
   <si>
     <t>channel-b</t>
   </si>
   <si>
-    <t>b-team</t>
-  </si>
-  <si>
-    <t>channel-a, channel-b, channel-c</t>
-  </si>
-  <si>
-    <t>team</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>channels</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>afirst</t>
+  </si>
+  <si>
+    <t>alast</t>
+  </si>
+  <si>
+    <t>bfirst</t>
+  </si>
+  <si>
+    <t>blast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,16 +113,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,66 +395,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>